<commit_message>
Se actualiza script NCD
</commit_message>
<xml_diff>
--- a/src/test/resources/data/excel/Data.xlsx
+++ b/src/test/resources/data/excel/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Orlando\Desktop\TSOFT\PROYECTOS\Mi Banco\mibanco_auto_app-framework-1.0.0\src\test\resources\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56453BE9-3801-48FD-913B-571D49BA7D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A64886-6AF9-4E06-9668-60FCFD9834F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="5190" windowWidth="18510" windowHeight="15015" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <sheet name="CancelacionCta" sheetId="12" r:id="rId6"/>
     <sheet name="TransferenciasOtrasCuentas" sheetId="9" r:id="rId7"/>
     <sheet name="TransferenciaEntreMisCuentas" sheetId="10" r:id="rId8"/>
-    <sheet name="Flujos" sheetId="8" r:id="rId9"/>
+    <sheet name="MiPerfil" sheetId="13" r:id="rId9"/>
+    <sheet name="DesembolsoEAT" sheetId="14" r:id="rId10"/>
+    <sheet name="Flujos" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="120">
   <si>
     <t>correo</t>
   </si>
@@ -116,9 +118,6 @@
     <t>Srvexqancd5@mibanco.com.pe</t>
   </si>
   <si>
-    <t>Ht-2Cdj(2ev</t>
-  </si>
-  <si>
     <t>Fe%eGT)1Y</t>
   </si>
   <si>
@@ -196,15 +195,6 @@
   </si>
   <si>
     <t>soles</t>
-  </si>
-  <si>
-    <t>Regresión  - Transferencia a Otras Cuentas APP - SOLES</t>
-  </si>
-  <si>
-    <t>Regresión  - Transferencia a Otras Cuentas APP - DOLARES</t>
-  </si>
-  <si>
-    <t>Regresión  - Transferencia entre mis Cuentas APP</t>
   </si>
   <si>
     <t>tipoCuenta</t>
@@ -255,9 +245,6 @@
     <t>Se realice el flujo de cancelacion de cuenta de manera correcta</t>
   </si>
   <si>
-    <t xml:space="preserve"> DATA LISTA</t>
-  </si>
-  <si>
     <t>DATA LISTA</t>
   </si>
   <si>
@@ -265,9 +252,6 @@
   </si>
   <si>
     <t>CASO18 - Regresión  - Apertura de Cuenta Correcto APP - AHORROS NEGOCIOS  DOLARES</t>
-  </si>
-  <si>
-    <t>CAMBIAR CORREO</t>
   </si>
   <si>
     <t>data lista</t>
@@ -295,25 +279,142 @@
 Cliente DNI</t>
   </si>
   <si>
-    <t>2AL_T3(DeR</t>
-  </si>
-  <si>
     <t>CASO4- Regresión  - Activacion modo de confirmacion por Correo</t>
   </si>
   <si>
-    <t>DATA LISTA DESPUES DE CONFIRMACION DE CORREO</t>
-  </si>
-  <si>
-    <t>saul2021</t>
-  </si>
-  <si>
-    <t>0312749856</t>
-  </si>
-  <si>
-    <t>0312761653</t>
-  </si>
-  <si>
     <t>cliente registrado</t>
+  </si>
+  <si>
+    <t>SqL780$Da</t>
+  </si>
+  <si>
+    <t>USUARIO</t>
+  </si>
+  <si>
+    <t>DISPLAY NAME</t>
+  </si>
+  <si>
+    <t>CLAVE</t>
+  </si>
+  <si>
+    <t>Srvexqancd1</t>
+  </si>
+  <si>
+    <t>NCD - Funcionalidad Registro con tarjeta</t>
+  </si>
+  <si>
+    <t>NqL670$Kd</t>
+  </si>
+  <si>
+    <t>Srvexqancd2</t>
+  </si>
+  <si>
+    <t>NCD- Funcionalidad: Olvide mi contraseña</t>
+  </si>
+  <si>
+    <t>Tu*$8734A</t>
+  </si>
+  <si>
+    <t>Srvexqancd3</t>
+  </si>
+  <si>
+    <t>NCD-Funcion:Activacion de token digital</t>
+  </si>
+  <si>
+    <t>Srvexqancd4</t>
+  </si>
+  <si>
+    <t>NCD- Funcionalidad:Perfil y cerrar sesion</t>
+  </si>
+  <si>
+    <t>Yo*$678A0</t>
+  </si>
+  <si>
+    <t>Srvexqancd5</t>
+  </si>
+  <si>
+    <t>NCD- Funcionalidad: Desembolsos</t>
+  </si>
+  <si>
+    <t>TpL09$4Ic</t>
+  </si>
+  <si>
+    <t>Srvexqancd6</t>
+  </si>
+  <si>
+    <t>NCD- Funcionalidad: Transferencias</t>
+  </si>
+  <si>
+    <t>Se*$803K4</t>
+  </si>
+  <si>
+    <t>Full ahorro (Soles)</t>
+  </si>
+  <si>
+    <t>Ahorro negocios (Dólares)</t>
+  </si>
+  <si>
+    <t>Regresión  - Transferencia entre mis Cuentas APP - SOLES A SOLES</t>
+  </si>
+  <si>
+    <t>Regresión  - Transferencia entre mis Cuentas APP - SOLES A DOLARES</t>
+  </si>
+  <si>
+    <t>Regresión  - Transferencia entre mis Cuentas APP - DOLARES A SOLES</t>
+  </si>
+  <si>
+    <t>Regresión  - Validacion de datos personales MiPerfil</t>
+  </si>
+  <si>
+    <t>Se realiza la correcta valdiacion de datos personales</t>
+  </si>
+  <si>
+    <t>CASO14 - Regresión  - Apertura de Cuenta Correcto APP - AHORROS NEGOCIOS  DOLARES</t>
+  </si>
+  <si>
+    <t>Se realice el flujo de desembolso EAT correctamente</t>
+  </si>
+  <si>
+    <t>Dia a Pagar</t>
+  </si>
+  <si>
+    <t>Motivo Prestamo</t>
+  </si>
+  <si>
+    <t>Cuotas</t>
+  </si>
+  <si>
+    <t>Compra de deuda</t>
+  </si>
+  <si>
+    <t>Seguro</t>
+  </si>
+  <si>
+    <t>Cuenta a Desembolsar</t>
+  </si>
+  <si>
+    <t>Regresión  - Transferencia entre mis Cuentas APP - DOLARES A DOLARES</t>
+  </si>
+  <si>
+    <t>Full ahorro (Dólares)</t>
+  </si>
+  <si>
+    <t>Regresión  - Transferencia a Otras Cuentas APP - SOLES A SOLES</t>
+  </si>
+  <si>
+    <t>Regresión  - Transferencia a Otras Cuentas APP - SOLES A DOLARES</t>
+  </si>
+  <si>
+    <t>Regresión  - Transferencia a Otras Cuentas APP - DOLARES A DOLARES</t>
+  </si>
+  <si>
+    <t>Regresión  - Transferencia a Otras Cuentas APP - DOLARES A SOLES</t>
+  </si>
+  <si>
+    <t>saul2020</t>
+  </si>
+  <si>
+    <t>0312139017</t>
   </si>
 </sst>
 </file>
@@ -407,7 +508,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -430,6 +531,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -437,7 +551,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -503,9 +617,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -529,6 +640,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -547,6 +674,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1085850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>524532</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>153842</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB3A507D-FEFF-7927-B52D-613318D64180}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="1628775"/>
+          <a:ext cx="4706007" cy="10336067"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>753210</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>39836</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9119DB4-666A-5D11-5708-0CE2ECA99C8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17516475" y="552450"/>
+          <a:ext cx="5268060" cy="12441386"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -815,7 +1035,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,10 +1094,10 @@
         <v>6</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="I2" s="6"/>
     </row>
@@ -901,10 +1121,10 @@
         <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="33.75" x14ac:dyDescent="0.25">
@@ -927,10 +1147,10 @@
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -962,12 +1182,442 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD9EAD1-7735-4C45-A120-F6F2895CC959}">
+  <dimension ref="A1:Q6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="16.42578125" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:17" s="29" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="40">
+        <v>59200076</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="29">
+        <v>900</v>
+      </c>
+      <c r="H2" s="29">
+        <v>25</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="29">
+        <v>12</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+    </row>
+    <row r="3" spans="1:17" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="9">
+        <v>49982697</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="29">
+        <v>2000</v>
+      </c>
+      <c r="H3" s="29">
+        <v>15</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="J3" s="29">
+        <v>6</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="32"/>
+    </row>
+    <row r="4" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="32"/>
+    </row>
+    <row r="5" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="32"/>
+    </row>
+    <row r="6" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="32"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{AF560E57-DB31-4765-B9B6-50334C5F4B1D}"/>
+    <hyperlink ref="M3" r:id="rId2" xr:uid="{AD61547C-D71B-4000-B4B7-0F1FA1F4CFC9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B849B470-D3A7-4ED1-BA05-D4DE0C628D81}">
+  <dimension ref="B2:D23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="13"/>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="11"/>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+    </row>
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D53FB81-1E32-442A-ACD1-3C0199CCE986}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,10 +1672,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>15</v>
@@ -1033,26 +1683,26 @@
       <c r="E2" s="24">
         <v>39854190</v>
       </c>
-      <c r="F2" s="28" t="s">
-        <v>74</v>
+      <c r="F2" s="27" t="s">
+        <v>68</v>
       </c>
       <c r="G2" s="25">
         <v>1111</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="L2" s="25" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M2" s="25">
         <v>1</v>
@@ -1063,10 +1713,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>15</v>
@@ -1084,16 +1734,16 @@
         <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="K3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1127,10 +1777,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00542B68-23CA-49C5-9D28-BAD7C19E85C4}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,9 +1793,10 @@
     <col min="9" max="9" width="20" customWidth="1"/>
     <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1179,34 +1830,37 @@
       <c r="K1" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="L1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E2" s="9">
-        <v>35462505</v>
+        <v>49982697</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="G2">
         <v>1111</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="J2" t="s">
         <v>6</v>
@@ -1215,36 +1869,34 @@
         <v>6</v>
       </c>
       <c r="L2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="M2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E3">
-        <v>17163572</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>85</v>
-      </c>
+      <c r="F3" s="36"/>
       <c r="G3">
         <v>1111</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="J3" t="s">
         <v>6</v>
@@ -1253,14 +1905,14 @@
         <v>6</v>
       </c>
       <c r="L3" t="s">
-        <v>86</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" xr:uid="{F70F2780-A2AB-44FD-8AD4-89B5DAA70C42}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{2EBBBA84-6D67-4746-93BF-39342A50E0DE}"/>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{D626BFB2-14F8-4630-99EA-641F2EEE024D}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{30A6D199-873E-49FB-B1BB-6C0043B0F4A3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1269,10 +1921,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F42D9C63-BC1D-44F8-95FB-6969FB103C9B}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="G3:H3"/>
+      <selection activeCell="E2" sqref="E2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,7 +1936,7 @@
     <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1310,265 +1962,102 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="25" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="25">
-        <v>39854190</v>
-      </c>
-      <c r="F2" s="25" t="s">
+    <row r="2" spans="1:9" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="9">
+        <v>49982697</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="J2" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="9">
-        <v>59200076</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="9">
-        <v>26441377</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="9">
-        <v>91188353</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="9">
-        <v>53367848</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="9">
-        <v>39582104</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="9">
-        <v>30417975</v>
-      </c>
-      <c r="F8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="9">
-        <v>22509645</v>
-      </c>
-      <c r="F9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="9">
-        <v>82449576</v>
-      </c>
-      <c r="F10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="9"/>
-      <c r="G12" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="9"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="9"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="9"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="9"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="9"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="9"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="9"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="9"/>
+      <c r="G11" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G10" r:id="rId1" xr:uid="{3F97AFA0-683C-49C1-8A6D-98234DB8C8F7}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{62EF13D3-3101-4DFB-9AE7-85378B373387}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{F09F1E15-E9F5-4CCA-83D1-7F68CE2E3EFE}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{5A6096F2-F912-4C3C-B455-65A07D16368C}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{CD9312C5-13A7-4E45-914D-5BE9B1757182}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{C92CDE69-07B5-4EBB-A800-5BCC2CF82053}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{A6CE97CF-B19B-4A10-ADA9-A6598AA92FBB}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{D2366B14-F673-48D3-AE4C-165FD962A431}"/>
-    <hyperlink ref="G2" r:id="rId9" xr:uid="{48389364-55E2-4094-9B26-2D5D0AF88E2A}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{4080F291-161D-44B5-A223-A3921F72AEAE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1576,10 +2065,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FA2929D-FE78-4FF4-B340-579630AD2C51}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,7 +2082,7 @@
     <col min="11" max="11" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1619,100 +2108,94 @@
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="31">
+        <v>59200076</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="32">
-        <v>59200076</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="J2" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="L2" s="33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="K2" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E3" s="25">
         <v>39854190</v>
       </c>
       <c r="F3" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="K3" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="L3" s="25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E4" s="1">
         <v>80024755</v>
@@ -1721,30 +2204,33 @@
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="K4" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E5" s="1">
         <v>84234339</v>
@@ -1753,30 +2239,33 @@
         <v>6</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="K5" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E6">
         <v>27310380</v>
@@ -1785,58 +2274,28 @@
         <v>6</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E7">
-        <v>27310380</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>57</v>
+      <c r="K6" s="32" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" xr:uid="{AA434A5E-18B4-4EA0-B6F9-A56BEE410614}"/>
-    <hyperlink ref="G7" r:id="rId2" xr:uid="{783EAF48-5911-427B-95B0-24AD06CE6645}"/>
-    <hyperlink ref="G6" r:id="rId3" xr:uid="{F2097A30-3C62-45F3-8ED1-4E264F6570D6}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{B5598C5C-4505-48BB-AD32-4B135DFA2FD8}"/>
-    <hyperlink ref="G2" r:id="rId5" xr:uid="{E6376C6C-8FB4-4D30-8E0A-B8D04899991F}"/>
-    <hyperlink ref="G3" r:id="rId6" xr:uid="{DC0F465D-8D47-4D43-8FC3-00A45A179B58}"/>
+    <hyperlink ref="G6" r:id="rId2" xr:uid="{F2097A30-3C62-45F3-8ED1-4E264F6570D6}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{B5598C5C-4505-48BB-AD32-4B135DFA2FD8}"/>
+    <hyperlink ref="G2" r:id="rId4" xr:uid="{E6376C6C-8FB4-4D30-8E0A-B8D04899991F}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{DC0F465D-8D47-4D43-8FC3-00A45A179B58}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1844,10 +2303,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726838D5-F96E-4066-9B72-DF4433B46C44}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,7 +2338,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>0</v>
@@ -1888,136 +2347,154 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="25" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E2" s="25">
+        <v>39854190</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2">
+        <v>6019396051</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="31">
+        <v>59200076</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="25" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="25">
         <v>27310380</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="25">
-        <v>6019394822</v>
-      </c>
-      <c r="H2" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" s="23" t="s">
+      <c r="G4" s="23"/>
+      <c r="H4" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="K2" s="25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="25" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="25">
-        <v>27310380</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="23">
-        <v>6019394792</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="K3" s="25">
+      <c r="J4" s="28"/>
+      <c r="K4" s="25">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="1">
-        <v>80024755</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E5" s="1">
-        <v>84234339</v>
+        <v>80024755</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="1">
+        <v>84234339</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" xr:uid="{1D05BADF-61D3-4836-BB2B-8A34E40D377F}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{CF1C0ACF-B24D-4CB9-A31C-A2F1A8CECA24}"/>
-    <hyperlink ref="H2" r:id="rId3" xr:uid="{34501533-419C-455C-B3CD-C5130CF2160F}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{E20E85AF-9359-4876-8622-1DD59B801297}"/>
+    <hyperlink ref="H5" r:id="rId1" xr:uid="{1D05BADF-61D3-4836-BB2B-8A34E40D377F}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{CF1C0ACF-B24D-4CB9-A31C-A2F1A8CECA24}"/>
+    <hyperlink ref="H6" r:id="rId3" xr:uid="{E20E85AF-9359-4876-8622-1DD59B801297}"/>
+    <hyperlink ref="H3" r:id="rId4" xr:uid="{6E1C8255-AED5-4E78-A8D8-ED56B6B4A844}"/>
+    <hyperlink ref="H2" r:id="rId5" xr:uid="{F67D8C0D-4D19-4C9A-9436-9A2C34050CC2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2025,10 +2502,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE255F87-8171-4A1B-9DFA-AE9CC5E0AC00}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,16 +2541,16 @@
         <v>3</v>
       </c>
       <c r="G1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="16" t="s">
-        <v>44</v>
-      </c>
       <c r="I1" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="16" t="s">
         <v>46</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>47</v>
       </c>
       <c r="K1" s="16" t="s">
         <v>0</v>
@@ -2082,47 +2559,47 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="33" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="31" t="s">
+    <row r="2" spans="1:14" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="34">
+      <c r="E2" s="33">
         <v>80024755</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="33">
+      <c r="G2" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="32">
         <v>6019195714</v>
       </c>
-      <c r="I2" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="36">
-        <v>1</v>
-      </c>
-      <c r="K2" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="L2" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="M2" s="33" t="s">
+      <c r="I2" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="35">
+        <v>5</v>
+      </c>
+      <c r="K2" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="N2" s="33">
+      <c r="L2" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" s="32">
         <v>3</v>
       </c>
     </row>
@@ -2131,13 +2608,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>51</v>
+        <v>115</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="E3" s="1">
         <v>80024755</v>
@@ -2146,36 +2623,106 @@
         <v>6</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3">
         <v>6018223846</v>
       </c>
       <c r="I3" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="19">
+        <v>1400</v>
+      </c>
+      <c r="K3" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="1">
+        <v>80024755</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4">
+        <v>6018223846</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="19">
+        <v>0.99</v>
+      </c>
+      <c r="K4" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="1">
+        <v>80024755</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="32">
+        <v>6019195714</v>
+      </c>
+      <c r="I5" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="19">
-        <v>15.3</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G4">
-        <v>6019308721</v>
+      <c r="J5" s="19">
+        <v>5001</v>
+      </c>
+      <c r="K5" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" xr:uid="{0DF3DB7E-A155-438A-A310-36B653CE1138}"/>
-    <hyperlink ref="K2" r:id="rId2" xr:uid="{63063CA1-B0C1-4670-8914-A93902747DEE}"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{63063CA1-B0C1-4670-8914-A93902747DEE}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{6694A830-EC45-42BE-9782-D25E961A608B}"/>
+    <hyperlink ref="K4" r:id="rId3" xr:uid="{DE7A5979-C40D-487F-9B89-4103F580FF7D}"/>
+    <hyperlink ref="K5" r:id="rId4" xr:uid="{8048EEDE-FFBC-48FA-9F85-08CF2B0D0F73}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2183,10 +2730,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD8DF1F-E487-45DB-9D4D-A795504229A2}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2197,12 +2744,12 @@
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.140625" customWidth="1"/>
     <col min="8" max="8" width="28.42578125" customWidth="1"/>
-    <col min="9" max="10" width="19.42578125" customWidth="1"/>
-    <col min="11" max="11" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2222,36 +2769,33 @@
         <v>3</v>
       </c>
       <c r="G1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>43</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>44</v>
       </c>
       <c r="I1" s="16" t="s">
         <v>46</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="1">
         <v>80024755</v>
@@ -2260,36 +2804,33 @@
         <v>6</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2">
-        <v>6019195714</v>
-      </c>
-      <c r="I2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="20">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="22.5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="20">
+        <v>50</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="E3" s="1">
         <v>80024755</v>
@@ -2298,151 +2839,175 @@
         <v>6</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3">
-        <v>6018223846</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="19">
-        <v>15.3</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G4">
-        <v>6019308721</v>
+        <v>44</v>
+      </c>
+      <c r="H3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="19">
+        <v>10</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="1">
+        <v>80024755</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="19">
+        <v>30</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="1">
+        <v>80024755</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I5" s="19">
+        <v>14</v>
+      </c>
+      <c r="J5" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" s="32" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" xr:uid="{DF692327-F5B8-4773-B74F-FCF4060F128A}"/>
-    <hyperlink ref="K2" r:id="rId2" xr:uid="{534DF8D7-9D4F-453F-A121-694295E4A82E}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{BE87599E-0F07-42DF-ACDB-1B7D7A34C724}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{611619E7-4750-45E2-9398-5F35CB9E4A49}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{4A5EA8BE-F8FF-4B16-9C03-361B7B327C29}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{AFFFCFBF-75AD-4D0B-A22F-A70C7E75EC95}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B849B470-D3A7-4ED1-BA05-D4DE0C628D81}">
-  <dimension ref="C2:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7895C4BE-30BE-4F53-9B8E-5DDA533787AA}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="13"/>
-    </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="11"/>
-    </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="13" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-    </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+      <c r="D2" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="1">
+        <v>80024755</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{70E098B6-8CBD-4D54-94DD-A0E6F0E3307D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>